<commit_message>
Updated mon stat spreadsheet
</commit_message>
<xml_diff>
--- a/MonStats.xlsx
+++ b/MonStats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\Godot\MonScript\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9D3A42A2-75DC-478E-B52B-8902620666C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0A7A411-10AE-44C0-B8B9-382EEE0CDF77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{423268FB-9D0F-495A-8574-C27E1B4A4DCB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Mon</t>
   </si>
@@ -126,6 +126,9 @@
   </si>
   <si>
     <t>SPD (X)</t>
+  </si>
+  <si>
+    <t>BIT2Kill (X)</t>
   </si>
 </sst>
 </file>
@@ -514,10 +517,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D949AA0-CB52-4B56-90E0-307ED24144A1}">
-  <dimension ref="A1:R10"/>
+  <dimension ref="A1:S10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -527,7 +530,7 @@
     <col min="16" max="16" width="14.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -570,14 +573,17 @@
       <c r="O1" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="P1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1">
+      <c r="S1">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -594,108 +600,116 @@
         <v>96</v>
       </c>
       <c r="F2" s="2">
-        <f t="shared" ref="F2:F3" si="0">ROUNDUP((B2*$R$6)+(C2*$R$7)+(D2*$R$8)+(E2*$R$9), 0)</f>
+        <f>ROUNDUP((B2*$S$6)+(C2*$S$7)+(D2*$S$8)+(E2*$S$9), 0)</f>
         <v>528</v>
       </c>
       <c r="G2" s="2">
-        <f>ROUNDDOWN(B2/($R$2+$R$1)*$R$1, 0)</f>
+        <f>ROUNDDOWN(B2/($S$2+$S$1)*$S$1, 0)</f>
         <v>34</v>
       </c>
       <c r="H2" s="2">
-        <f>ROUNDDOWN(C2/($R$2+$R$1)*$R$1, 0)</f>
+        <f>ROUNDDOWN(C2/($S$2+$S$1)*$S$1, 0)</f>
         <v>17</v>
       </c>
       <c r="I2" s="2">
-        <f>ROUNDDOWN(D2/($R$2+$R$1)*$R$1, 0)</f>
+        <f>ROUNDDOWN(D2/($S$2+$S$1)*$S$1, 0)</f>
         <v>8</v>
       </c>
       <c r="J2" s="2">
-        <f>ROUNDDOWN(E2/($R$2+$R$1)*$R$1, 0)</f>
+        <f>ROUNDDOWN(E2/($S$2+$S$1)*$S$1, 0)</f>
         <v>12</v>
       </c>
       <c r="L2" s="2">
-        <f>ROUNDDOWN(($R$3/$R$2)*(B2-G2)+G2, 0)</f>
-        <v>34</v>
+        <f>ROUNDDOWN(($S$3/$S$2)*(B2-G2)+G2, 0)</f>
+        <v>256</v>
       </c>
       <c r="M2" s="2">
-        <f>ROUNDDOWN(($R$3/$R$2)*(C2-H2)+H2, 0)</f>
+        <f>ROUNDDOWN(($S$3/$S$2)*(C2-H2)+H2, 0)</f>
+        <v>128</v>
+      </c>
+      <c r="N2" s="2">
+        <f>ROUNDDOWN(($S$3/$S$2)*(D2-I2)+I2, 0)</f>
+        <v>64</v>
+      </c>
+      <c r="O2" s="2">
+        <f>ROUNDDOWN(($S$3/$S$2)*(E2-J2)+J2, 0)</f>
+        <v>96</v>
+      </c>
+      <c r="P2" s="2">
+        <f>ROUNDUP(L2/($M$2-N2), 0)</f>
+        <v>4</v>
+      </c>
+      <c r="R2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="N2" s="2">
-        <f>ROUNDDOWN(($R$3/$R$2)*(D2-I2)+I2, 0)</f>
-        <v>8</v>
-      </c>
-      <c r="O2" s="2">
-        <f>ROUNDDOWN(($R$3/$R$2)*(E2-J2)+J2, 0)</f>
-        <v>12</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="R2">
+      <c r="S2">
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="3">
-        <v>660</v>
+        <v>540</v>
       </c>
       <c r="C3" s="3">
-        <v>55</v>
+        <v>98</v>
       </c>
       <c r="D3" s="3">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E3" s="3">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="F3" s="2">
-        <f t="shared" si="0"/>
-        <v>534</v>
+        <f>ROUNDUP((B3*$S$6)+(C3*$S$7)+(D3*$S$8)+(E3*$S$9), 0)</f>
+        <v>507</v>
       </c>
       <c r="G3" s="2">
-        <f>ROUNDDOWN(B3/($R$2+$R$1)*$R$1, 0)</f>
-        <v>89</v>
+        <f>ROUNDDOWN(B3/($S$2+$S$1)*$S$1, 0)</f>
+        <v>72</v>
       </c>
       <c r="H3" s="2">
-        <f>ROUNDDOWN(C3/($R$2+$R$1)*$R$1, 0)</f>
-        <v>7</v>
+        <f>ROUNDDOWN(C3/($S$2+$S$1)*$S$1, 0)</f>
+        <v>13</v>
       </c>
       <c r="I3" s="2">
-        <f>ROUNDDOWN(D3/($R$2+$R$1)*$R$1, 0)</f>
-        <v>2</v>
+        <f>ROUNDDOWN(D3/($S$2+$S$1)*$S$1, 0)</f>
+        <v>1</v>
       </c>
       <c r="J3" s="2">
-        <f>ROUNDDOWN(E3/($R$2+$R$1)*$R$1, 0)</f>
+        <f>ROUNDDOWN(E3/($S$2+$S$1)*$S$1, 0)</f>
         <v>10</v>
       </c>
       <c r="L3" s="2">
-        <f>ROUNDDOWN(($R$3/$R$2)*(B3-G3)+G3, 0)</f>
-        <v>89</v>
+        <f>ROUNDDOWN(($S$3/$S$2)*(B3-G3)+G3, 0)</f>
+        <v>540</v>
       </c>
       <c r="M3" s="2">
-        <f>ROUNDDOWN(($R$3/$R$2)*(C3-H3)+H3, 0)</f>
-        <v>7</v>
+        <f>ROUNDDOWN(($S$3/$S$2)*(C3-H3)+H3, 0)</f>
+        <v>98</v>
       </c>
       <c r="N3" s="2">
-        <f>ROUNDDOWN(($R$3/$R$2)*(D3-I3)+I3, 0)</f>
-        <v>2</v>
+        <f>ROUNDDOWN(($S$3/$S$2)*(D3-I3)+I3, 0)</f>
+        <v>14</v>
       </c>
       <c r="O3" s="2">
-        <f>ROUNDDOWN(($R$3/$R$2)*(E3-J3)+J3, 0)</f>
-        <v>10</v>
-      </c>
-      <c r="Q3" s="1" t="s">
+        <f>ROUNDDOWN(($S$3/$S$2)*(E3-J3)+J3, 0)</f>
+        <v>74</v>
+      </c>
+      <c r="P3" s="2">
+        <f t="shared" ref="P3:P10" si="0">ROUNDUP(L3/($M$2-N3), 0)</f>
+        <v>5</v>
+      </c>
+      <c r="R3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="R3">
-        <v>0</v>
+      <c r="S3">
+        <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -712,43 +726,47 @@
         <v>95</v>
       </c>
       <c r="F4" s="2">
-        <f>ROUNDUP((B4*$R$6)+(C4*$R$7)+(D4*$R$8)+(E4*$R$9), 0)</f>
+        <f>ROUNDUP((B4*$S$6)+(C4*$S$7)+(D4*$S$8)+(E4*$S$9), 0)</f>
         <v>437</v>
       </c>
       <c r="G4" s="2">
-        <f>ROUNDDOWN(B4/($R$2+$R$1)*$R$1, 0)</f>
+        <f>ROUNDDOWN(B4/($S$2+$S$1)*$S$1, 0)</f>
         <v>29</v>
       </c>
       <c r="H4" s="2">
-        <f>ROUNDDOWN(C4/($R$2+$R$1)*$R$1, 0)</f>
+        <f>ROUNDDOWN(C4/($S$2+$S$1)*$S$1, 0)</f>
         <v>13</v>
       </c>
       <c r="I4" s="2">
-        <f>ROUNDDOWN(D4/($R$2+$R$1)*$R$1, 0)</f>
+        <f>ROUNDDOWN(D4/($S$2+$S$1)*$S$1, 0)</f>
         <v>5</v>
       </c>
       <c r="J4" s="2">
-        <f>ROUNDDOWN(E4/($R$2+$R$1)*$R$1, 0)</f>
+        <f>ROUNDDOWN(E4/($S$2+$S$1)*$S$1, 0)</f>
         <v>12</v>
       </c>
       <c r="L4" s="2">
-        <f>ROUNDDOWN(($R$3/$R$2)*(B4-G4)+G4, 0)</f>
-        <v>29</v>
+        <f>ROUNDDOWN(($S$3/$S$2)*(B4-G4)+G4, 0)</f>
+        <v>220</v>
       </c>
       <c r="M4" s="2">
-        <f>ROUNDDOWN(($R$3/$R$2)*(C4-H4)+H4, 0)</f>
-        <v>13</v>
+        <f>ROUNDDOWN(($S$3/$S$2)*(C4-H4)+H4, 0)</f>
+        <v>100</v>
       </c>
       <c r="N4" s="2">
-        <f>ROUNDDOWN(($R$3/$R$2)*(D4-I4)+I4, 0)</f>
-        <v>5</v>
+        <f>ROUNDDOWN(($S$3/$S$2)*(D4-I4)+I4, 0)</f>
+        <v>42</v>
       </c>
       <c r="O4" s="2">
-        <f>ROUNDDOWN(($R$3/$R$2)*(E4-J4)+J4, 0)</f>
-        <v>12</v>
+        <f>ROUNDDOWN(($S$3/$S$2)*(E4-J4)+J4, 0)</f>
+        <v>95</v>
+      </c>
+      <c r="P4" s="2">
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>19</v>
       </c>
@@ -756,7 +774,7 @@
         <v>220</v>
       </c>
       <c r="C5" s="3">
-        <v>145</v>
+        <v>158</v>
       </c>
       <c r="D5" s="3">
         <v>42</v>
@@ -765,43 +783,47 @@
         <v>135</v>
       </c>
       <c r="F5" s="2">
-        <f t="shared" ref="F5:F10" si="1">ROUNDUP((B5*$R$6)+(C5*$R$7)+(D5*$R$8)+(E5*$R$9), 0)</f>
-        <v>542</v>
+        <f>ROUNDUP((B5*$S$6)+(C5*$S$7)+(D5*$S$8)+(E5*$S$9), 0)</f>
+        <v>555</v>
       </c>
       <c r="G5" s="2">
-        <f>ROUNDDOWN(B5/($R$2+$R$1)*$R$1, 0)</f>
+        <f>ROUNDDOWN(B5/($S$2+$S$1)*$S$1, 0)</f>
         <v>29</v>
       </c>
       <c r="H5" s="2">
-        <f>ROUNDDOWN(C5/($R$2+$R$1)*$R$1, 0)</f>
-        <v>19</v>
+        <f>ROUNDDOWN(C5/($S$2+$S$1)*$S$1, 0)</f>
+        <v>21</v>
       </c>
       <c r="I5" s="2">
-        <f>ROUNDDOWN(D5/($R$2+$R$1)*$R$1, 0)</f>
+        <f>ROUNDDOWN(D5/($S$2+$S$1)*$S$1, 0)</f>
         <v>5</v>
       </c>
       <c r="J5" s="2">
-        <f>ROUNDDOWN(E5/($R$2+$R$1)*$R$1, 0)</f>
+        <f>ROUNDDOWN(E5/($S$2+$S$1)*$S$1, 0)</f>
         <v>18</v>
       </c>
       <c r="L5" s="2">
-        <f>ROUNDDOWN(($R$3/$R$2)*(B5-G5)+G5, 0)</f>
-        <v>29</v>
+        <f>ROUNDDOWN(($S$3/$S$2)*(B5-G5)+G5, 0)</f>
+        <v>220</v>
       </c>
       <c r="M5" s="2">
-        <f>ROUNDDOWN(($R$3/$R$2)*(C5-H5)+H5, 0)</f>
-        <v>19</v>
+        <f>ROUNDDOWN(($S$3/$S$2)*(C5-H5)+H5, 0)</f>
+        <v>158</v>
       </c>
       <c r="N5" s="2">
-        <f>ROUNDDOWN(($R$3/$R$2)*(D5-I5)+I5, 0)</f>
-        <v>5</v>
+        <f>ROUNDDOWN(($S$3/$S$2)*(D5-I5)+I5, 0)</f>
+        <v>42</v>
       </c>
       <c r="O5" s="2">
-        <f>ROUNDDOWN(($R$3/$R$2)*(E5-J5)+J5, 0)</f>
-        <v>18</v>
+        <f>ROUNDDOWN(($S$3/$S$2)*(E5-J5)+J5, 0)</f>
+        <v>135</v>
+      </c>
+      <c r="P5" s="2">
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -818,167 +840,179 @@
         <v>28</v>
       </c>
       <c r="F6" s="2">
-        <f t="shared" si="1"/>
+        <f>ROUNDUP((B6*$S$6)+(C6*$S$7)+(D6*$S$8)+(E6*$S$9), 0)</f>
         <v>480</v>
       </c>
       <c r="G6" s="2">
-        <f>ROUNDDOWN(B6/($R$2+$R$1)*$R$1, 0)</f>
+        <f>ROUNDDOWN(B6/($S$2+$S$1)*$S$1, 0)</f>
         <v>44</v>
       </c>
       <c r="H6" s="2">
-        <f>ROUNDDOWN(C6/($R$2+$R$1)*$R$1, 0)</f>
+        <f>ROUNDDOWN(C6/($S$2+$S$1)*$S$1, 0)</f>
         <v>13</v>
       </c>
       <c r="I6" s="2">
-        <f>ROUNDDOWN(D6/($R$2+$R$1)*$R$1, 0)</f>
+        <f>ROUNDDOWN(D6/($S$2+$S$1)*$S$1, 0)</f>
         <v>11</v>
       </c>
       <c r="J6" s="2">
-        <f>ROUNDDOWN(E6/($R$2+$R$1)*$R$1, 0)</f>
+        <f>ROUNDDOWN(E6/($S$2+$S$1)*$S$1, 0)</f>
         <v>3</v>
       </c>
       <c r="L6" s="2">
-        <f>ROUNDDOWN(($R$3/$R$2)*(B6-G6)+G6, 0)</f>
-        <v>44</v>
+        <f>ROUNDDOWN(($S$3/$S$2)*(B6-G6)+G6, 0)</f>
+        <v>328</v>
       </c>
       <c r="M6" s="2">
-        <f>ROUNDDOWN(($R$3/$R$2)*(C6-H6)+H6, 0)</f>
-        <v>13</v>
+        <f>ROUNDDOWN(($S$3/$S$2)*(C6-H6)+H6, 0)</f>
+        <v>98</v>
       </c>
       <c r="N6" s="2">
-        <f>ROUNDDOWN(($R$3/$R$2)*(D6-I6)+I6, 0)</f>
-        <v>11</v>
+        <f>ROUNDDOWN(($S$3/$S$2)*(D6-I6)+I6, 0)</f>
+        <v>88</v>
       </c>
       <c r="O6" s="2">
-        <f>ROUNDDOWN(($R$3/$R$2)*(E6-J6)+J6, 0)</f>
-        <v>3</v>
-      </c>
-      <c r="Q6" s="1" t="s">
+        <f>ROUNDDOWN(($S$3/$S$2)*(E6-J6)+J6, 0)</f>
+        <v>28</v>
+      </c>
+      <c r="P6" s="2">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="R6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="R6">
+      <c r="S6">
         <v>0.5</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B7" s="3">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="C7" s="3">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D7" s="3">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E7" s="3">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="F7" s="2">
-        <f t="shared" si="1"/>
-        <v>487</v>
+        <f>ROUNDUP((B7*$S$6)+(C7*$S$7)+(D7*$S$8)+(E7*$S$9), 0)</f>
+        <v>500</v>
       </c>
       <c r="G7" s="2">
-        <f>ROUNDDOWN(B7/($R$2+$R$1)*$R$1, 0)</f>
+        <f>ROUNDDOWN(B7/($S$2+$S$1)*$S$1, 0)</f>
         <v>28</v>
       </c>
       <c r="H7" s="2">
-        <f>ROUNDDOWN(C7/($R$2+$R$1)*$R$1, 0)</f>
+        <f>ROUNDDOWN(C7/($S$2+$S$1)*$S$1, 0)</f>
         <v>19</v>
       </c>
       <c r="I7" s="2">
-        <f>ROUNDDOWN(D7/($R$2+$R$1)*$R$1, 0)</f>
-        <v>8</v>
+        <f>ROUNDDOWN(D7/($S$2+$S$1)*$S$1, 0)</f>
+        <v>7</v>
       </c>
       <c r="J7" s="2">
-        <f>ROUNDDOWN(E7/($R$2+$R$1)*$R$1, 0)</f>
-        <v>10</v>
+        <f>ROUNDDOWN(E7/($S$2+$S$1)*$S$1, 0)</f>
+        <v>12</v>
       </c>
       <c r="L7" s="2">
-        <f>ROUNDDOWN(($R$3/$R$2)*(B7-G7)+G7, 0)</f>
-        <v>28</v>
+        <f>ROUNDDOWN(($S$3/$S$2)*(B7-G7)+G7, 0)</f>
+        <v>212</v>
       </c>
       <c r="M7" s="2">
-        <f>ROUNDDOWN(($R$3/$R$2)*(C7-H7)+H7, 0)</f>
-        <v>19</v>
+        <f>ROUNDDOWN(($S$3/$S$2)*(C7-H7)+H7, 0)</f>
+        <v>144</v>
       </c>
       <c r="N7" s="2">
-        <f>ROUNDDOWN(($R$3/$R$2)*(D7-I7)+I7, 0)</f>
-        <v>8</v>
+        <f>ROUNDDOWN(($S$3/$S$2)*(D7-I7)+I7, 0)</f>
+        <v>58</v>
       </c>
       <c r="O7" s="2">
-        <f>ROUNDDOWN(($R$3/$R$2)*(E7-J7)+J7, 0)</f>
-        <v>10</v>
-      </c>
-      <c r="Q7" s="1" t="s">
+        <f>ROUNDDOWN(($S$3/$S$2)*(E7-J7)+J7, 0)</f>
+        <v>89</v>
+      </c>
+      <c r="P7" s="2">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="R7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="R7">
+      <c r="S7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="3">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="C8" s="3">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="D8" s="3">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="E8" s="3">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="F8" s="2">
-        <f t="shared" si="1"/>
-        <v>462</v>
+        <f>ROUNDUP((B8*$S$6)+(C8*$S$7)+(D8*$S$8)+(E8*$S$9), 0)</f>
+        <v>484</v>
       </c>
       <c r="G8" s="2">
-        <f>ROUNDDOWN(B8/($R$2+$R$1)*$R$1, 0)</f>
+        <f>ROUNDDOWN(B8/($S$2+$S$1)*$S$1, 0)</f>
         <v>26</v>
       </c>
       <c r="H8" s="2">
-        <f>ROUNDDOWN(C8/($R$2+$R$1)*$R$1, 0)</f>
-        <v>17</v>
+        <f>ROUNDDOWN(C8/($S$2+$S$1)*$S$1, 0)</f>
+        <v>15</v>
       </c>
       <c r="I8" s="2">
-        <f>ROUNDDOWN(D8/($R$2+$R$1)*$R$1, 0)</f>
-        <v>10</v>
+        <f>ROUNDDOWN(D8/($S$2+$S$1)*$S$1, 0)</f>
+        <v>11</v>
       </c>
       <c r="J8" s="2">
-        <f>ROUNDDOWN(E8/($R$2+$R$1)*$R$1, 0)</f>
-        <v>7</v>
+        <f>ROUNDDOWN(E8/($S$2+$S$1)*$S$1, 0)</f>
+        <v>8</v>
       </c>
       <c r="L8" s="2">
-        <f>ROUNDDOWN(($R$3/$R$2)*(B8-G8)+G8, 0)</f>
-        <v>26</v>
+        <f>ROUNDDOWN(($S$3/$S$2)*(B8-G8)+G8, 0)</f>
+        <v>198</v>
       </c>
       <c r="M8" s="2">
-        <f>ROUNDDOWN(($R$3/$R$2)*(C8-H8)+H8, 0)</f>
-        <v>17</v>
+        <f>ROUNDDOWN(($S$3/$S$2)*(C8-H8)+H8, 0)</f>
+        <v>115</v>
       </c>
       <c r="N8" s="2">
-        <f>ROUNDDOWN(($R$3/$R$2)*(D8-I8)+I8, 0)</f>
-        <v>10</v>
+        <f>ROUNDDOWN(($S$3/$S$2)*(D8-I8)+I8, 0)</f>
+        <v>86</v>
       </c>
       <c r="O8" s="2">
-        <f>ROUNDDOWN(($R$3/$R$2)*(E8-J8)+J8, 0)</f>
-        <v>7</v>
-      </c>
-      <c r="Q8" s="1" t="s">
+        <f>ROUNDDOWN(($S$3/$S$2)*(E8-J8)+J8, 0)</f>
+        <v>65</v>
+      </c>
+      <c r="P8" s="2">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="R8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="R8">
+      <c r="S8">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>6</v>
       </c>
@@ -995,99 +1029,107 @@
         <v>126</v>
       </c>
       <c r="F9" s="2">
-        <f t="shared" si="1"/>
+        <f>ROUNDUP((B9*$S$6)+(C9*$S$7)+(D9*$S$8)+(E9*$S$9), 0)</f>
         <v>490</v>
       </c>
       <c r="G9" s="2">
-        <f>ROUNDDOWN(B9/($R$2+$R$1)*$R$1, 0)</f>
+        <f>ROUNDDOWN(B9/($S$2+$S$1)*$S$1, 0)</f>
         <v>28</v>
       </c>
       <c r="H9" s="2">
-        <f>ROUNDDOWN(C9/($R$2+$R$1)*$R$1, 0)</f>
+        <f>ROUNDDOWN(C9/($S$2+$S$1)*$S$1, 0)</f>
         <v>11</v>
       </c>
       <c r="I9" s="2">
-        <f>ROUNDDOWN(D9/($R$2+$R$1)*$R$1, 0)</f>
+        <f>ROUNDDOWN(D9/($S$2+$S$1)*$S$1, 0)</f>
         <v>7</v>
       </c>
       <c r="J9" s="2">
-        <f>ROUNDDOWN(E9/($R$2+$R$1)*$R$1, 0)</f>
+        <f>ROUNDDOWN(E9/($S$2+$S$1)*$S$1, 0)</f>
         <v>17</v>
       </c>
       <c r="L9" s="2">
-        <f>ROUNDDOWN(($R$3/$R$2)*(B9-G9)+G9, 0)</f>
-        <v>28</v>
+        <f>ROUNDDOWN(($S$3/$S$2)*(B9-G9)+G9, 0)</f>
+        <v>210</v>
       </c>
       <c r="M9" s="2">
-        <f>ROUNDDOWN(($R$3/$R$2)*(C9-H9)+H9, 0)</f>
-        <v>11</v>
+        <f>ROUNDDOWN(($S$3/$S$2)*(C9-H9)+H9, 0)</f>
+        <v>84</v>
       </c>
       <c r="N9" s="2">
-        <f>ROUNDDOWN(($R$3/$R$2)*(D9-I9)+I9, 0)</f>
-        <v>7</v>
+        <f>ROUNDDOWN(($S$3/$S$2)*(D9-I9)+I9, 0)</f>
+        <v>56</v>
       </c>
       <c r="O9" s="2">
-        <f>ROUNDDOWN(($R$3/$R$2)*(E9-J9)+J9, 0)</f>
-        <v>17</v>
-      </c>
-      <c r="Q9" s="1" t="s">
+        <f>ROUNDDOWN(($S$3/$S$2)*(E9-J9)+J9, 0)</f>
+        <v>126</v>
+      </c>
+      <c r="P9" s="2">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="R9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="R9">
+      <c r="S9">
         <v>1.5</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="3">
-        <v>320</v>
+        <v>328</v>
       </c>
       <c r="C10" s="3">
         <v>170</v>
       </c>
       <c r="D10" s="3">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="E10" s="3">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="F10" s="2">
-        <f t="shared" si="1"/>
-        <v>502</v>
+        <f>ROUNDUP((B10*$S$6)+(C10*$S$7)+(D10*$S$8)+(E10*$S$9), 0)</f>
+        <v>511</v>
       </c>
       <c r="G10" s="2">
-        <f>ROUNDDOWN(B10/($R$2+$R$1)*$R$1, 0)</f>
-        <v>43</v>
+        <f>ROUNDDOWN(B10/($S$2+$S$1)*$S$1, 0)</f>
+        <v>44</v>
       </c>
       <c r="H10" s="2">
-        <f>ROUNDDOWN(C10/($R$2+$R$1)*$R$1, 0)</f>
+        <f>ROUNDDOWN(C10/($S$2+$S$1)*$S$1, 0)</f>
         <v>22</v>
       </c>
       <c r="I10" s="2">
-        <f>ROUNDDOWN(D10/($R$2+$R$1)*$R$1, 0)</f>
+        <f>ROUNDDOWN(D10/($S$2+$S$1)*$S$1, 0)</f>
+        <v>5</v>
+      </c>
+      <c r="J10" s="2">
+        <f>ROUNDDOWN(E10/($S$2+$S$1)*$S$1, 0)</f>
+        <v>7</v>
+      </c>
+      <c r="L10" s="2">
+        <f>ROUNDDOWN(($S$3/$S$2)*(B10-G10)+G10, 0)</f>
+        <v>328</v>
+      </c>
+      <c r="M10" s="2">
+        <f>ROUNDDOWN(($S$3/$S$2)*(C10-H10)+H10, 0)</f>
+        <v>170</v>
+      </c>
+      <c r="N10" s="2">
+        <f>ROUNDDOWN(($S$3/$S$2)*(D10-I10)+I10, 0)</f>
+        <v>44</v>
+      </c>
+      <c r="O10" s="2">
+        <f>ROUNDDOWN(($S$3/$S$2)*(E10-J10)+J10, 0)</f>
+        <v>59</v>
+      </c>
+      <c r="P10" s="2">
+        <f t="shared" si="0"/>
         <v>4</v>
-      </c>
-      <c r="J10" s="2">
-        <f>ROUNDDOWN(E10/($R$2+$R$1)*$R$1, 0)</f>
-        <v>9</v>
-      </c>
-      <c r="L10" s="2">
-        <f>ROUNDDOWN(($R$3/$R$2)*(B10-G10)+G10, 0)</f>
-        <v>43</v>
-      </c>
-      <c r="M10" s="2">
-        <f>ROUNDDOWN(($R$3/$R$2)*(C10-H10)+H10, 0)</f>
-        <v>22</v>
-      </c>
-      <c r="N10" s="2">
-        <f>ROUNDDOWN(($R$3/$R$2)*(D10-I10)+I10, 0)</f>
-        <v>4</v>
-      </c>
-      <c r="O10" s="2">
-        <f>ROUNDDOWN(($R$3/$R$2)*(E10-J10)+J10, 0)</f>
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated mon spreadsheet a bit; modified mondata to use new formulas; fixed mondata tests
</commit_message>
<xml_diff>
--- a/MonStats.xlsx
+++ b/MonStats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\Godot\MonScript\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0A7A411-10AE-44C0-B8B9-382EEE0CDF77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1517E4C-8267-4874-93D6-175DD50B78F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{423268FB-9D0F-495A-8574-C27E1B4A4DCB}"/>
+    <workbookView xWindow="76800" yWindow="10500" windowWidth="19200" windowHeight="21000" xr2:uid="{423268FB-9D0F-495A-8574-C27E1B4A4DCB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -517,10 +517,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D949AA0-CB52-4B56-90E0-307ED24144A1}">
-  <dimension ref="A1:S10"/>
+  <dimension ref="A1:S23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -600,44 +600,44 @@
         <v>96</v>
       </c>
       <c r="F2" s="2">
-        <f>ROUNDUP((B2*$S$6)+(C2*$S$7)+(D2*$S$8)+(E2*$S$9), 0)</f>
+        <f t="shared" ref="F2:F10" si="0">ROUNDUP((B2*$S$6)+(C2*$S$7)+(D2*$S$8)+(E2*$S$9), 0)</f>
         <v>528</v>
       </c>
       <c r="G2" s="2">
-        <f>ROUNDDOWN(B2/($S$2+$S$1)*$S$1, 0)</f>
+        <f t="shared" ref="G2:G10" si="1">ROUNDDOWN(B2/($S$2+$S$1)*$S$1, 0)</f>
         <v>34</v>
       </c>
       <c r="H2" s="2">
-        <f>ROUNDDOWN(C2/($S$2+$S$1)*$S$1, 0)</f>
+        <f t="shared" ref="H2:H10" si="2">ROUNDDOWN(C2/($S$2+$S$1)*$S$1, 0)</f>
         <v>17</v>
       </c>
       <c r="I2" s="2">
-        <f>ROUNDDOWN(D2/($S$2+$S$1)*$S$1, 0)</f>
+        <f t="shared" ref="I2:I10" si="3">ROUNDDOWN(D2/($S$2+$S$1)*$S$1, 0)</f>
         <v>8</v>
       </c>
       <c r="J2" s="2">
-        <f>ROUNDDOWN(E2/($S$2+$S$1)*$S$1, 0)</f>
+        <f t="shared" ref="J2:J10" si="4">ROUNDDOWN(E2/($S$2+$S$1)*$S$1, 0)</f>
         <v>12</v>
       </c>
       <c r="L2" s="2">
-        <f>ROUNDDOWN(($S$3/$S$2)*(B2-G2)+G2, 0)</f>
-        <v>256</v>
+        <f>ROUNDUP(($S$3/$S$2)*(B2-G2)+G2, 0)</f>
+        <v>41</v>
       </c>
       <c r="M2" s="2">
-        <f>ROUNDDOWN(($S$3/$S$2)*(C2-H2)+H2, 0)</f>
-        <v>128</v>
+        <f t="shared" ref="M2:P2" si="5">ROUNDUP(($S$3/$S$2)*(C2-H2)+H2, 0)</f>
+        <v>21</v>
       </c>
       <c r="N2" s="2">
-        <f>ROUNDDOWN(($S$3/$S$2)*(D2-I2)+I2, 0)</f>
-        <v>64</v>
+        <f t="shared" si="5"/>
+        <v>10</v>
       </c>
       <c r="O2" s="2">
-        <f>ROUNDDOWN(($S$3/$S$2)*(E2-J2)+J2, 0)</f>
-        <v>96</v>
+        <f t="shared" si="5"/>
+        <v>15</v>
       </c>
       <c r="P2" s="2">
-        <f>ROUNDUP(L2/($M$2-N2), 0)</f>
-        <v>4</v>
+        <f t="shared" si="5"/>
+        <v>17</v>
       </c>
       <c r="R2" s="1" t="s">
         <v>17</v>
@@ -663,50 +663,50 @@
         <v>74</v>
       </c>
       <c r="F3" s="2">
-        <f>ROUNDUP((B3*$S$6)+(C3*$S$7)+(D3*$S$8)+(E3*$S$9), 0)</f>
+        <f t="shared" si="0"/>
         <v>507</v>
       </c>
       <c r="G3" s="2">
-        <f>ROUNDDOWN(B3/($S$2+$S$1)*$S$1, 0)</f>
+        <f t="shared" si="1"/>
         <v>72</v>
       </c>
       <c r="H3" s="2">
-        <f>ROUNDDOWN(C3/($S$2+$S$1)*$S$1, 0)</f>
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
       <c r="I3" s="2">
-        <f>ROUNDDOWN(D3/($S$2+$S$1)*$S$1, 0)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J3" s="2">
-        <f>ROUNDDOWN(E3/($S$2+$S$1)*$S$1, 0)</f>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="L3" s="2">
-        <f>ROUNDDOWN(($S$3/$S$2)*(B3-G3)+G3, 0)</f>
-        <v>540</v>
+        <f t="shared" ref="L3:L10" si="6">ROUNDUP(($S$3/$S$2)*(B3-G3)+G3, 0)</f>
+        <v>87</v>
       </c>
       <c r="M3" s="2">
-        <f>ROUNDDOWN(($S$3/$S$2)*(C3-H3)+H3, 0)</f>
-        <v>98</v>
+        <f t="shared" ref="M3:M10" si="7">ROUNDUP(($S$3/$S$2)*(C3-H3)+H3, 0)</f>
+        <v>16</v>
       </c>
       <c r="N3" s="2">
-        <f>ROUNDDOWN(($S$3/$S$2)*(D3-I3)+I3, 0)</f>
-        <v>14</v>
+        <f t="shared" ref="N3:N10" si="8">ROUNDUP(($S$3/$S$2)*(D3-I3)+I3, 0)</f>
+        <v>2</v>
       </c>
       <c r="O3" s="2">
-        <f>ROUNDDOWN(($S$3/$S$2)*(E3-J3)+J3, 0)</f>
-        <v>74</v>
+        <f t="shared" ref="O3:O10" si="9">ROUNDUP(($S$3/$S$2)*(E3-J3)+J3, 0)</f>
+        <v>12</v>
       </c>
       <c r="P3" s="2">
-        <f t="shared" ref="P3:P10" si="0">ROUNDUP(L3/($M$2-N3), 0)</f>
-        <v>5</v>
+        <f t="shared" ref="P3:P10" si="10">ROUNDUP(($S$3/$S$2)*(F3-K3)+K3, 0)</f>
+        <v>16</v>
       </c>
       <c r="R3" s="1" t="s">
         <v>26</v>
       </c>
       <c r="S3">
-        <v>64</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.35">
@@ -726,44 +726,44 @@
         <v>95</v>
       </c>
       <c r="F4" s="2">
-        <f>ROUNDUP((B4*$S$6)+(C4*$S$7)+(D4*$S$8)+(E4*$S$9), 0)</f>
+        <f t="shared" si="0"/>
         <v>437</v>
       </c>
       <c r="G4" s="2">
-        <f>ROUNDDOWN(B4/($S$2+$S$1)*$S$1, 0)</f>
+        <f t="shared" si="1"/>
         <v>29</v>
       </c>
       <c r="H4" s="2">
-        <f>ROUNDDOWN(C4/($S$2+$S$1)*$S$1, 0)</f>
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
       <c r="I4" s="2">
-        <f>ROUNDDOWN(D4/($S$2+$S$1)*$S$1, 0)</f>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="J4" s="2">
-        <f>ROUNDDOWN(E4/($S$2+$S$1)*$S$1, 0)</f>
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
       <c r="L4" s="2">
-        <f>ROUNDDOWN(($S$3/$S$2)*(B4-G4)+G4, 0)</f>
-        <v>220</v>
+        <f t="shared" si="6"/>
+        <v>35</v>
       </c>
       <c r="M4" s="2">
-        <f>ROUNDDOWN(($S$3/$S$2)*(C4-H4)+H4, 0)</f>
-        <v>100</v>
+        <f t="shared" si="7"/>
+        <v>16</v>
       </c>
       <c r="N4" s="2">
-        <f>ROUNDDOWN(($S$3/$S$2)*(D4-I4)+I4, 0)</f>
-        <v>42</v>
+        <f t="shared" si="8"/>
+        <v>7</v>
       </c>
       <c r="O4" s="2">
-        <f>ROUNDDOWN(($S$3/$S$2)*(E4-J4)+J4, 0)</f>
-        <v>95</v>
+        <f t="shared" si="9"/>
+        <v>15</v>
       </c>
       <c r="P4" s="2">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f t="shared" si="10"/>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.35">
@@ -783,44 +783,44 @@
         <v>135</v>
       </c>
       <c r="F5" s="2">
-        <f>ROUNDUP((B5*$S$6)+(C5*$S$7)+(D5*$S$8)+(E5*$S$9), 0)</f>
+        <f t="shared" si="0"/>
         <v>555</v>
       </c>
       <c r="G5" s="2">
-        <f>ROUNDDOWN(B5/($S$2+$S$1)*$S$1, 0)</f>
+        <f t="shared" si="1"/>
         <v>29</v>
       </c>
       <c r="H5" s="2">
-        <f>ROUNDDOWN(C5/($S$2+$S$1)*$S$1, 0)</f>
+        <f t="shared" si="2"/>
         <v>21</v>
       </c>
       <c r="I5" s="2">
-        <f>ROUNDDOWN(D5/($S$2+$S$1)*$S$1, 0)</f>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="J5" s="2">
-        <f>ROUNDDOWN(E5/($S$2+$S$1)*$S$1, 0)</f>
+        <f t="shared" si="4"/>
         <v>18</v>
       </c>
       <c r="L5" s="2">
-        <f>ROUNDDOWN(($S$3/$S$2)*(B5-G5)+G5, 0)</f>
-        <v>220</v>
+        <f t="shared" si="6"/>
+        <v>35</v>
       </c>
       <c r="M5" s="2">
-        <f>ROUNDDOWN(($S$3/$S$2)*(C5-H5)+H5, 0)</f>
-        <v>158</v>
+        <f t="shared" si="7"/>
+        <v>26</v>
       </c>
       <c r="N5" s="2">
-        <f>ROUNDDOWN(($S$3/$S$2)*(D5-I5)+I5, 0)</f>
-        <v>42</v>
+        <f t="shared" si="8"/>
+        <v>7</v>
       </c>
       <c r="O5" s="2">
-        <f>ROUNDDOWN(($S$3/$S$2)*(E5-J5)+J5, 0)</f>
-        <v>135</v>
+        <f t="shared" si="9"/>
+        <v>22</v>
       </c>
       <c r="P5" s="2">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f t="shared" si="10"/>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.35">
@@ -840,44 +840,44 @@
         <v>28</v>
       </c>
       <c r="F6" s="2">
-        <f>ROUNDUP((B6*$S$6)+(C6*$S$7)+(D6*$S$8)+(E6*$S$9), 0)</f>
+        <f t="shared" si="0"/>
         <v>480</v>
       </c>
       <c r="G6" s="2">
-        <f>ROUNDDOWN(B6/($S$2+$S$1)*$S$1, 0)</f>
+        <f t="shared" si="1"/>
         <v>44</v>
       </c>
       <c r="H6" s="2">
-        <f>ROUNDDOWN(C6/($S$2+$S$1)*$S$1, 0)</f>
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
       <c r="I6" s="2">
-        <f>ROUNDDOWN(D6/($S$2+$S$1)*$S$1, 0)</f>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="J6" s="2">
-        <f>ROUNDDOWN(E6/($S$2+$S$1)*$S$1, 0)</f>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="L6" s="2">
-        <f>ROUNDDOWN(($S$3/$S$2)*(B6-G6)+G6, 0)</f>
-        <v>328</v>
+        <f t="shared" si="6"/>
+        <v>53</v>
       </c>
       <c r="M6" s="2">
-        <f>ROUNDDOWN(($S$3/$S$2)*(C6-H6)+H6, 0)</f>
-        <v>98</v>
+        <f t="shared" si="7"/>
+        <v>16</v>
       </c>
       <c r="N6" s="2">
-        <f>ROUNDDOWN(($S$3/$S$2)*(D6-I6)+I6, 0)</f>
-        <v>88</v>
+        <f t="shared" si="8"/>
+        <v>14</v>
       </c>
       <c r="O6" s="2">
-        <f>ROUNDDOWN(($S$3/$S$2)*(E6-J6)+J6, 0)</f>
-        <v>28</v>
+        <f t="shared" si="9"/>
+        <v>4</v>
       </c>
       <c r="P6" s="2">
-        <f t="shared" si="0"/>
-        <v>9</v>
+        <f t="shared" si="10"/>
+        <v>15</v>
       </c>
       <c r="R6" s="1" t="s">
         <v>21</v>
@@ -903,44 +903,44 @@
         <v>89</v>
       </c>
       <c r="F7" s="2">
-        <f>ROUNDUP((B7*$S$6)+(C7*$S$7)+(D7*$S$8)+(E7*$S$9), 0)</f>
+        <f t="shared" si="0"/>
         <v>500</v>
       </c>
       <c r="G7" s="2">
-        <f>ROUNDDOWN(B7/($S$2+$S$1)*$S$1, 0)</f>
+        <f t="shared" si="1"/>
         <v>28</v>
       </c>
       <c r="H7" s="2">
-        <f>ROUNDDOWN(C7/($S$2+$S$1)*$S$1, 0)</f>
+        <f t="shared" si="2"/>
         <v>19</v>
       </c>
       <c r="I7" s="2">
-        <f>ROUNDDOWN(D7/($S$2+$S$1)*$S$1, 0)</f>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="J7" s="2">
-        <f>ROUNDDOWN(E7/($S$2+$S$1)*$S$1, 0)</f>
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
       <c r="L7" s="2">
-        <f>ROUNDDOWN(($S$3/$S$2)*(B7-G7)+G7, 0)</f>
-        <v>212</v>
+        <f t="shared" si="6"/>
+        <v>34</v>
       </c>
       <c r="M7" s="2">
-        <f>ROUNDDOWN(($S$3/$S$2)*(C7-H7)+H7, 0)</f>
-        <v>144</v>
+        <f t="shared" si="7"/>
+        <v>23</v>
       </c>
       <c r="N7" s="2">
-        <f>ROUNDDOWN(($S$3/$S$2)*(D7-I7)+I7, 0)</f>
-        <v>58</v>
+        <f t="shared" si="8"/>
+        <v>9</v>
       </c>
       <c r="O7" s="2">
-        <f>ROUNDDOWN(($S$3/$S$2)*(E7-J7)+J7, 0)</f>
-        <v>89</v>
+        <f t="shared" si="9"/>
+        <v>15</v>
       </c>
       <c r="P7" s="2">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <f t="shared" si="10"/>
+        <v>16</v>
       </c>
       <c r="R7" s="1" t="s">
         <v>22</v>
@@ -966,44 +966,44 @@
         <v>65</v>
       </c>
       <c r="F8" s="2">
-        <f>ROUNDUP((B8*$S$6)+(C8*$S$7)+(D8*$S$8)+(E8*$S$9), 0)</f>
+        <f t="shared" si="0"/>
         <v>484</v>
       </c>
       <c r="G8" s="2">
-        <f>ROUNDDOWN(B8/($S$2+$S$1)*$S$1, 0)</f>
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="H8" s="2">
-        <f>ROUNDDOWN(C8/($S$2+$S$1)*$S$1, 0)</f>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="I8" s="2">
-        <f>ROUNDDOWN(D8/($S$2+$S$1)*$S$1, 0)</f>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="J8" s="2">
-        <f>ROUNDDOWN(E8/($S$2+$S$1)*$S$1, 0)</f>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="L8" s="2">
-        <f>ROUNDDOWN(($S$3/$S$2)*(B8-G8)+G8, 0)</f>
-        <v>198</v>
+        <f t="shared" si="6"/>
+        <v>32</v>
       </c>
       <c r="M8" s="2">
-        <f>ROUNDDOWN(($S$3/$S$2)*(C8-H8)+H8, 0)</f>
-        <v>115</v>
+        <f t="shared" si="7"/>
+        <v>19</v>
       </c>
       <c r="N8" s="2">
-        <f>ROUNDDOWN(($S$3/$S$2)*(D8-I8)+I8, 0)</f>
-        <v>86</v>
+        <f t="shared" si="8"/>
+        <v>14</v>
       </c>
       <c r="O8" s="2">
-        <f>ROUNDDOWN(($S$3/$S$2)*(E8-J8)+J8, 0)</f>
-        <v>65</v>
+        <f t="shared" si="9"/>
+        <v>10</v>
       </c>
       <c r="P8" s="2">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <f t="shared" si="10"/>
+        <v>16</v>
       </c>
       <c r="R8" s="1" t="s">
         <v>23</v>
@@ -1029,44 +1029,44 @@
         <v>126</v>
       </c>
       <c r="F9" s="2">
-        <f>ROUNDUP((B9*$S$6)+(C9*$S$7)+(D9*$S$8)+(E9*$S$9), 0)</f>
+        <f t="shared" si="0"/>
         <v>490</v>
       </c>
       <c r="G9" s="2">
-        <f>ROUNDDOWN(B9/($S$2+$S$1)*$S$1, 0)</f>
+        <f t="shared" si="1"/>
         <v>28</v>
       </c>
       <c r="H9" s="2">
-        <f>ROUNDDOWN(C9/($S$2+$S$1)*$S$1, 0)</f>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="I9" s="2">
-        <f>ROUNDDOWN(D9/($S$2+$S$1)*$S$1, 0)</f>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="J9" s="2">
-        <f>ROUNDDOWN(E9/($S$2+$S$1)*$S$1, 0)</f>
+        <f t="shared" si="4"/>
         <v>17</v>
       </c>
       <c r="L9" s="2">
-        <f>ROUNDDOWN(($S$3/$S$2)*(B9-G9)+G9, 0)</f>
-        <v>210</v>
+        <f t="shared" si="6"/>
+        <v>34</v>
       </c>
       <c r="M9" s="2">
-        <f>ROUNDDOWN(($S$3/$S$2)*(C9-H9)+H9, 0)</f>
-        <v>84</v>
+        <f t="shared" si="7"/>
+        <v>14</v>
       </c>
       <c r="N9" s="2">
-        <f>ROUNDDOWN(($S$3/$S$2)*(D9-I9)+I9, 0)</f>
-        <v>56</v>
+        <f t="shared" si="8"/>
+        <v>9</v>
       </c>
       <c r="O9" s="2">
-        <f>ROUNDDOWN(($S$3/$S$2)*(E9-J9)+J9, 0)</f>
-        <v>126</v>
+        <f t="shared" si="9"/>
+        <v>21</v>
       </c>
       <c r="P9" s="2">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f t="shared" si="10"/>
+        <v>16</v>
       </c>
       <c r="R9" s="1" t="s">
         <v>24</v>
@@ -1092,44 +1092,54 @@
         <v>59</v>
       </c>
       <c r="F10" s="2">
-        <f>ROUNDUP((B10*$S$6)+(C10*$S$7)+(D10*$S$8)+(E10*$S$9), 0)</f>
+        <f t="shared" si="0"/>
         <v>511</v>
       </c>
       <c r="G10" s="2">
-        <f>ROUNDDOWN(B10/($S$2+$S$1)*$S$1, 0)</f>
+        <f t="shared" si="1"/>
         <v>44</v>
       </c>
       <c r="H10" s="2">
-        <f>ROUNDDOWN(C10/($S$2+$S$1)*$S$1, 0)</f>
+        <f t="shared" si="2"/>
         <v>22</v>
       </c>
       <c r="I10" s="2">
-        <f>ROUNDDOWN(D10/($S$2+$S$1)*$S$1, 0)</f>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="J10" s="2">
-        <f>ROUNDDOWN(E10/($S$2+$S$1)*$S$1, 0)</f>
+        <f t="shared" si="4"/>
         <v>7</v>
       </c>
       <c r="L10" s="2">
-        <f>ROUNDDOWN(($S$3/$S$2)*(B10-G10)+G10, 0)</f>
-        <v>328</v>
+        <f t="shared" si="6"/>
+        <v>53</v>
       </c>
       <c r="M10" s="2">
-        <f>ROUNDDOWN(($S$3/$S$2)*(C10-H10)+H10, 0)</f>
-        <v>170</v>
+        <f t="shared" si="7"/>
+        <v>27</v>
       </c>
       <c r="N10" s="2">
-        <f>ROUNDDOWN(($S$3/$S$2)*(D10-I10)+I10, 0)</f>
-        <v>44</v>
+        <f t="shared" si="8"/>
+        <v>7</v>
       </c>
       <c r="O10" s="2">
-        <f>ROUNDDOWN(($S$3/$S$2)*(E10-J10)+J10, 0)</f>
-        <v>59</v>
+        <f t="shared" si="9"/>
+        <v>9</v>
       </c>
       <c r="P10" s="2">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <f t="shared" si="10"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="6:7" x14ac:dyDescent="0.35">
+      <c r="F23">
+        <f>256/(64+10)</f>
+        <v>3.4594594594594597</v>
+      </c>
+      <c r="G23">
+        <f>F23*10</f>
+        <v>34.594594594594597</v>
       </c>
     </row>
   </sheetData>

</xml_diff>